<commit_message>
dix: change calculate prices
</commit_message>
<xml_diff>
--- a/src/assets/modelo_crear_producto.xlsx
+++ b/src/assets/modelo_crear_producto.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27612"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="535" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18B4A72C-BE70-4E16-948D-7FCCDC0E91DE}"/>
+  <xr:revisionPtr revIDLastSave="540" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08BED413-72F2-41DC-9C72-BD31FEE18F91}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Orden </t>
   </si>
@@ -45,6 +45,9 @@
     <t>Marca</t>
   </si>
   <si>
+    <t>Padre rubro</t>
+  </si>
+  <si>
     <t>Rubro</t>
   </si>
   <si>
@@ -109,6 +112,9 @@
   </si>
   <si>
     <t>m3</t>
+  </si>
+  <si>
+    <t>Código Prov</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,31 +517,31 @@
     <col min="1" max="1" width="13.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" customWidth="1"/>
-    <col min="19" max="19" width="26.140625" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" customWidth="1"/>
-    <col min="22" max="22" width="35.28515625" customWidth="1"/>
-    <col min="23" max="23" width="14" customWidth="1"/>
-    <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" customWidth="1"/>
+    <col min="23" max="23" width="35.28515625" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -560,34 +566,34 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
@@ -605,43 +611,51 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Z1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="B2" s="7"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="3"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:26">
-      <c r="L3" s="3"/>
+    <row r="3" spans="1:28">
+      <c r="M3" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576 Q1:Q1048576 H1 I1 R1:R1048576 F1:F1048576 S1 V1 W1 X1 Y1 U1 T1 L1" xr:uid="{8FC600A4-ACC5-4C0D-B959-79AF7FF75442}"/>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{30C1A99E-F467-44F0-851E-89D1E5C3E2F5}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576 R1:R1048576 I1 J1 S1:S1048576 G1:G1048576 T1 W1 X1 Y1 Z1 V1 U1 M1" xr:uid="{8FC600A4-ACC5-4C0D-B959-79AF7FF75442}"/>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{30C1A99E-F467-44F0-851E-89D1E5C3E2F5}">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{BAF94131-F39D-4A72-98CC-2ECC201CAC9B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{BAF94131-F39D-4A72-98CC-2ECC201CAC9B}">
       <formula1>"Mostrador, Etiqueta, Cocina, Bar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576 U2:U1048576 Y2:Y1048576 X2:X1048576 V2:V1048576 W2:W1048576 T2:T1048576" xr:uid="{061FB7EB-430C-4567-ABE4-0EC758331A9B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576 V2:V1048576 Z2:Z1048576 Y2:Y1048576 W2:W1048576 X2:X1048576 U2:U1048576" xr:uid="{061FB7EB-430C-4567-ABE4-0EC758331A9B}">
       <formula1>"Si, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{720D906C-366B-433C-91EF-5227BFA3B28F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{720D906C-366B-433C-91EF-5227BFA3B28F}">
       <formula1>"gramos,kilogramos, kilómetros, litros, metros, metros cuadrados, metros cúbicos, unidad"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{BFC160FD-78C7-4BA3-BCCA-DB2719CE5BEA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{BFC160FD-78C7-4BA3-BCCA-DB2719CE5BEA}">
       <formula1>"21, 0, 27, 10.5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>